<commit_message>
EV-103 Create config downloadable file for VT application, add party logo in the export
</commit_message>
<xml_diff>
--- a/data/nrsr_2020/parties.xlsx
+++ b/data/nrsr_2020/parties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FIIT\tp\server\data\nrsr_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7451EA-8533-421D-BA7E-573491A65CFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D93CCB-6E78-4ABF-8DDB-CB7B85EBCD6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33135" yWindow="2040" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
   <si>
     <t>Číslo politického subjektu</t>
   </si>
@@ -157,6 +157,84 @@
   </si>
   <si>
     <t>ĽS Naše Slovensko</t>
+  </si>
+  <si>
+    <t>slovenska-ludova-strana-andreja-hlinku.png</t>
+  </si>
+  <si>
+    <t>dobra-volba.png</t>
+  </si>
+  <si>
+    <t>sloboda-a-solidarita.png</t>
+  </si>
+  <si>
+    <t>sme-rodina.png</t>
+  </si>
+  <si>
+    <t>slovenske-hnutie-obrody.png</t>
+  </si>
+  <si>
+    <t>za-ludi.png</t>
+  </si>
+  <si>
+    <t>mame-toho-dost.png</t>
+  </si>
+  <si>
+    <t>hlas-pravice.png</t>
+  </si>
+  <si>
+    <t>slovenska-narodna-strana.png</t>
+  </si>
+  <si>
+    <t>demokraticka-strana.png</t>
+  </si>
+  <si>
+    <t>obycajni-ludia-a-nezavisle-osobnosti.png</t>
+  </si>
+  <si>
+    <t>progresivne-slovensko-a-spolu.png</t>
+  </si>
+  <si>
+    <t>starostovia-a-nezavisli-kandidati.png</t>
+  </si>
+  <si>
+    <t>obciansky-hlas.png</t>
+  </si>
+  <si>
+    <t>krestanskodemokraticke-hnutie.png</t>
+  </si>
+  <si>
+    <t>slovenska-liga.png</t>
+  </si>
+  <si>
+    <t>vlast.png</t>
+  </si>
+  <si>
+    <t>most-hid.png</t>
+  </si>
+  <si>
+    <t>smer-socialna-demokracia.png</t>
+  </si>
+  <si>
+    <t>solidarita-hnutie-pracujucej-chudoby.png</t>
+  </si>
+  <si>
+    <t>hlas-ludu.png</t>
+  </si>
+  <si>
+    <t>madarska-komunitna-spolupatricnost.png</t>
+  </si>
+  <si>
+    <t>praca-slovenskeho-naroda.png</t>
+  </si>
+  <si>
+    <t>kotlebovci-ludova-strana-nase-slovensko.png</t>
+  </si>
+  <si>
+    <t>socialisti.png</t>
+  </si>
+  <si>
+    <t>image</t>
   </si>
 </sst>
 </file>
@@ -706,7 +784,10 @@
     <cellStyle name="Zvýraznenie5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Zvýraznenie6" xfId="38" builtinId="49" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -731,27 +812,29 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternéÚdaje_2" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="6">
-    <queryTableFields count="5">
+  <queryTableRefresh nextId="7" unboundColumnsRight="1">
+    <queryTableFields count="6">
       <queryTableField id="1" name="Číslo politického subjektu" tableColumnId="1"/>
       <queryTableField id="2" name="Názov politického subjektu" tableColumnId="2"/>
       <queryTableField id="3" name="Oficiálna skratka politického subjektu" tableColumnId="3"/>
       <queryTableField id="4" name="Počet kandidátov" tableColumnId="4"/>
       <queryTableField id="5" name="Poznámka" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PAR_2020_tab0a" displayName="PAR_2020_tab0a" ref="A1:E26" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E26" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PAR_2020_tab0a" displayName="PAR_2020_tab0a" ref="A1:F26" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F26" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Číslo politického subjektu" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Názov politického subjektu" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Oficiálna skratka politického subjektu" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Názov politického subjektu" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Oficiálna skratka politického subjektu" queryTableFieldId="3" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Počet kandidátov" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Poznámka" queryTableFieldId="5" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Poznámka" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{40C4F99E-B77A-405B-AF27-1CE4DA32FF5C}" uniqueName="6" name="image" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1054,9 +1137,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1064,10 +1149,11 @@
     <col min="2" max="2" width="77.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1083,8 +1169,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1100,8 +1189,11 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1117,8 +1209,11 @@
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1134,8 +1229,11 @@
       <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1151,8 +1249,11 @@
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1168,8 +1269,11 @@
       <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1185,8 +1289,11 @@
       <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1202,8 +1309,11 @@
       <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1219,8 +1329,11 @@
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1236,8 +1349,11 @@
       <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1253,8 +1369,11 @@
       <c r="E11" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1270,8 +1389,11 @@
       <c r="E12" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1287,8 +1409,11 @@
       <c r="E13" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1304,8 +1429,11 @@
       <c r="E14" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1321,8 +1449,11 @@
       <c r="E15" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1338,8 +1469,11 @@
       <c r="E16" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1355,8 +1489,11 @@
       <c r="E17" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1372,8 +1509,11 @@
       <c r="E18" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1389,8 +1529,11 @@
       <c r="E19" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1406,8 +1549,11 @@
       <c r="E20" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1423,8 +1569,11 @@
       <c r="E21" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1440,8 +1589,11 @@
       <c r="E22" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1457,8 +1609,11 @@
       <c r="E23" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1474,8 +1629,11 @@
       <c r="E24" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1491,8 +1649,11 @@
       <c r="E25" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1507,6 +1668,9 @@
       </c>
       <c r="E26" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EV-23 Add color to party import data, different probability for votes seeding, elastic returns now ids instead of names, helper lookup function
</commit_message>
<xml_diff>
--- a/data/nrsr_2020/parties.xlsx
+++ b/data/nrsr_2020/parties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FIIT\tp\server\data\nrsr_2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis/code/tp/server/data/nrsr_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D93CCB-6E78-4ABF-8DDB-CB7B85EBCD6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B97099-9A88-7E4F-8D39-91BBB0FE4F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33135" yWindow="2040" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
   <si>
     <t>Číslo politického subjektu</t>
   </si>
@@ -235,13 +235,91 @@
   </si>
   <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>#BED62F</t>
+  </si>
+  <si>
+    <t>#A70202</t>
+  </si>
+  <si>
+    <t>#0F4D92</t>
+  </si>
+  <si>
+    <t>#00521E</t>
+  </si>
+  <si>
+    <t>#015FB8</t>
+  </si>
+  <si>
+    <t>#96C82D</t>
+  </si>
+  <si>
+    <t>#FFCC00</t>
+  </si>
+  <si>
+    <t>#00528c</t>
+  </si>
+  <si>
+    <t>#009910</t>
+  </si>
+  <si>
+    <t>#062751</t>
+  </si>
+  <si>
+    <t>#FF0000</t>
+  </si>
+  <si>
+    <t>#014667</t>
+  </si>
+  <si>
+    <t>#FF8C00</t>
+  </si>
+  <si>
+    <t>#204198</t>
+  </si>
+  <si>
+    <t>#Fa2215</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>#5aa2D0</t>
+  </si>
+  <si>
+    <t>#A50020</t>
+  </si>
+  <si>
+    <t>#EE1D23</t>
+  </si>
+  <si>
+    <t>#B61737</t>
+  </si>
+  <si>
+    <t>#316F98</t>
+  </si>
+  <si>
+    <t>#DE1F26</t>
+  </si>
+  <si>
+    <t>#E0433F</t>
+  </si>
+  <si>
+    <t>#00008B</t>
+  </si>
+  <si>
+    <t>#376CB3</t>
+  </si>
+  <si>
+    <t>Farba</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +471,18 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE8EAED"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -736,55 +826,71 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - zvýraznenie1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - zvýraznenie2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - zvýraznenie3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - zvýraznenie4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - zvýraznenie5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - zvýraznenie6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - zvýraznenie1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - zvýraznenie2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - zvýraznenie3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - zvýraznenie4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - zvýraznenie5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - zvýraznenie6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - zvýraznenie1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - zvýraznenie2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - zvýraznenie3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - zvýraznenie4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - zvýraznenie5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - zvýraznenie6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Dobrá" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Kontrolná bunka" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Nadpis 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Nadpis 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Nadpis 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Nadpis 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Názov" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Neutrálna" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
-    <cellStyle name="Poznámka" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Prepojená bunka" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Spolu" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Text upozornenia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Vstup" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Výpočet" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Výstup" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Vysvetľujúci text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Zlá" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Zvýraznenie1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Zvýraznenie2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Zvýraznenie3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Zvýraznenie4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Zvýraznenie5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Zvýraznenie6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -812,36 +918,38 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternéÚdaje_2" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="7" unboundColumnsRight="1">
-    <queryTableFields count="6">
+  <queryTableRefresh nextId="8" unboundColumnsRight="2">
+    <queryTableFields count="7">
       <queryTableField id="1" name="Číslo politického subjektu" tableColumnId="1"/>
       <queryTableField id="2" name="Názov politického subjektu" tableColumnId="2"/>
       <queryTableField id="3" name="Oficiálna skratka politického subjektu" tableColumnId="3"/>
       <queryTableField id="4" name="Počet kandidátov" tableColumnId="4"/>
       <queryTableField id="5" name="Poznámka" tableColumnId="5"/>
       <queryTableField id="6" dataBound="0" tableColumnId="6"/>
+      <queryTableField id="7" dataBound="0" tableColumnId="7"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PAR_2020_tab0a" displayName="PAR_2020_tab0a" ref="A1:F26" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F26" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PAR_2020_tab0a" displayName="PAR_2020_tab0a" ref="A1:G26" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G26" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Číslo politického subjektu" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Názov politického subjektu" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Oficiálna skratka politického subjektu" queryTableFieldId="3" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Názov politického subjektu" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Oficiálna skratka politického subjektu" queryTableFieldId="3" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Počet kandidátov" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Poznámka" queryTableFieldId="5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{40C4F99E-B77A-405B-AF27-1CE4DA32FF5C}" uniqueName="6" name="image" queryTableFieldId="6" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Poznámka" queryTableFieldId="5" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{40C4F99E-B77A-405B-AF27-1CE4DA32FF5C}" uniqueName="6" name="image" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{E807A2C5-2799-1341-AAD3-DE9F0F207977}" uniqueName="7" name="Farba" queryTableFieldId="7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1137,23 +1245,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="49" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1172,8 +1281,11 @@
       <c r="F1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1192,8 +1304,11 @@
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1212,8 +1327,11 @@
       <c r="F3" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1232,8 +1350,11 @@
       <c r="F4" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1252,8 +1373,11 @@
       <c r="F5" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1272,8 +1396,11 @@
       <c r="F6" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1292,8 +1419,11 @@
       <c r="F7" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1312,8 +1442,11 @@
       <c r="F8" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1332,8 +1465,11 @@
       <c r="F9" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1352,8 +1488,11 @@
       <c r="F10" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1372,8 +1511,11 @@
       <c r="F11" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1392,8 +1534,12 @@
       <c r="F12" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1412,8 +1558,11 @@
       <c r="F13" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1432,8 +1581,11 @@
       <c r="F14" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1452,8 +1604,11 @@
       <c r="F15" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1472,8 +1627,11 @@
       <c r="F16" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1492,8 +1650,11 @@
       <c r="F17" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1512,8 +1673,11 @@
       <c r="F18" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1532,8 +1696,11 @@
       <c r="F19" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1552,8 +1719,11 @@
       <c r="F20" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1572,8 +1742,11 @@
       <c r="F21" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1592,8 +1765,11 @@
       <c r="F22" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1612,8 +1788,11 @@
       <c r="F23" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1632,8 +1811,11 @@
       <c r="F24" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1652,8 +1834,11 @@
       <c r="F25" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1671,6 +1856,9 @@
       </c>
       <c r="F26" s="1" t="s">
         <v>65</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EV-141 Add party abbr for seeding
</commit_message>
<xml_diff>
--- a/data/nrsr_2020/parties.xlsx
+++ b/data/nrsr_2020/parties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis/code/tp/server/data/nrsr_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B97099-9A88-7E4F-8D39-91BBB0FE4F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569839B4-0B7D-124A-8D40-FBA2F7FA6BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
   <si>
     <t>Číslo politického subjektu</t>
   </si>
@@ -313,13 +313,61 @@
   </si>
   <si>
     <t>Farba</t>
+  </si>
+  <si>
+    <t>Skratka</t>
+  </si>
+  <si>
+    <t>HLAS PRAV</t>
+  </si>
+  <si>
+    <t>OĽANO</t>
+  </si>
+  <si>
+    <t>SMER-SD</t>
+  </si>
+  <si>
+    <t>ĽSNS</t>
+  </si>
+  <si>
+    <t>PS SPOLU</t>
+  </si>
+  <si>
+    <t>SOCIALISTI</t>
+  </si>
+  <si>
+    <t>SOLIDARITA</t>
+  </si>
+  <si>
+    <t>MKO-MKS</t>
+  </si>
+  <si>
+    <t>MOST-HID</t>
+  </si>
+  <si>
+    <t>SLOV. LIGA</t>
+  </si>
+  <si>
+    <t>STANK</t>
+  </si>
+  <si>
+    <t>SĽS</t>
+  </si>
+  <si>
+    <t>SAS</t>
+  </si>
+  <si>
+    <t>SHO</t>
+  </si>
+  <si>
+    <t>MÁME TOHO DOSŤ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,12 +519,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFE8EAED"/>
-      <name val="Menlo"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -826,13 +868,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -878,7 +921,19 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -918,8 +973,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternéÚdaje_2" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="8" unboundColumnsRight="2">
-    <queryTableFields count="7">
+  <queryTableRefresh nextId="9" unboundColumnsRight="3">
+    <queryTableFields count="8">
       <queryTableField id="1" name="Číslo politického subjektu" tableColumnId="1"/>
       <queryTableField id="2" name="Názov politického subjektu" tableColumnId="2"/>
       <queryTableField id="3" name="Oficiálna skratka politického subjektu" tableColumnId="3"/>
@@ -927,22 +982,24 @@
       <queryTableField id="5" name="Poznámka" tableColumnId="5"/>
       <queryTableField id="6" dataBound="0" tableColumnId="6"/>
       <queryTableField id="7" dataBound="0" tableColumnId="7"/>
+      <queryTableField id="8" dataBound="0" tableColumnId="8"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PAR_2020_tab0a" displayName="PAR_2020_tab0a" ref="A1:G26" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G26" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PAR_2020_tab0a" displayName="PAR_2020_tab0a" ref="A1:H26" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H26" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Číslo politického subjektu" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Názov politického subjektu" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Oficiálna skratka politického subjektu" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Názov politického subjektu" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Oficiálna skratka politického subjektu" queryTableFieldId="3" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Počet kandidátov" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Poznámka" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{40C4F99E-B77A-405B-AF27-1CE4DA32FF5C}" uniqueName="6" name="image" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{E807A2C5-2799-1341-AAD3-DE9F0F207977}" uniqueName="7" name="Farba" queryTableFieldId="7" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Poznámka" queryTableFieldId="5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{40C4F99E-B77A-405B-AF27-1CE4DA32FF5C}" uniqueName="6" name="image" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{E807A2C5-2799-1341-AAD3-DE9F0F207977}" uniqueName="7" name="Farba" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{D593BA0C-E992-1843-B4CC-34ADB33C68FC}" uniqueName="8" name="Skratka" queryTableFieldId="8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1247,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1259,7 +1316,8 @@
     <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="49" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1281,8 +1339,11 @@
       <c r="F1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>92</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1304,8 +1365,11 @@
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>80</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1327,8 +1391,11 @@
       <c r="F3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>77</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1350,8 +1417,11 @@
       <c r="F4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1373,8 +1443,11 @@
       <c r="F5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>69</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1396,8 +1469,11 @@
       <c r="F6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>81</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1419,8 +1495,11 @@
       <c r="F7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>73</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1442,8 +1521,11 @@
       <c r="F8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>82</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1465,8 +1547,11 @@
       <c r="F9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>91</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1488,8 +1573,11 @@
       <c r="F10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>76</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1511,8 +1599,11 @@
       <c r="F11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>90</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1534,10 +1625,12 @@
       <c r="F12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1558,8 +1651,11 @@
       <c r="F13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>71</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1581,8 +1677,11 @@
       <c r="F14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>83</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1604,8 +1703,11 @@
       <c r="F15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>84</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0.99</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1627,11 +1729,14 @@
       <c r="F16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1650,11 +1755,14 @@
       <c r="F17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1673,11 +1781,14 @@
       <c r="F18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1696,11 +1807,14 @@
       <c r="F19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1719,11 +1833,14 @@
       <c r="F20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1742,11 +1859,14 @@
       <c r="F21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1765,11 +1885,14 @@
       <c r="F22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1788,11 +1911,14 @@
       <c r="F23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1811,11 +1937,14 @@
       <c r="F24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1834,11 +1963,14 @@
       <c r="F25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1857,8 +1989,11 @@
       <c r="F26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>89</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EV-184 change colors and probabilities of seeding
</commit_message>
<xml_diff>
--- a/data/nrsr_2020/parties.xlsx
+++ b/data/nrsr_2020/parties.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis/code/tp/server/data/nrsr_2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tp\server\data\nrsr_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569839B4-0B7D-124A-8D40-FBA2F7FA6BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="756" windowWidth="30240" windowHeight="18876"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -23,11 +22,11 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Dotaz – PAR_2020_tab0a" description="Pripojenie k dotazu PAR_2020_tab0a v zošite." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="Dotaz – PAR_2020_tab0a" description="Pripojenie k dotazu PAR_2020_tab0a v zošite." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=PAR_2020_tab0a;Extended Properties=&quot;&quot;" command="SELECT * FROM [PAR_2020_tab0a]"/>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="Dotaz – PAR_2020_tab0b" description="Pripojenie k dotazu PAR_2020_tab0b v zošite." type="5" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" keepAlive="1" name="Dotaz – PAR_2020_tab0b" description="Pripojenie k dotazu PAR_2020_tab0b v zošite." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=PAR_2020_tab0b;Extended Properties=&quot;&quot;" command="SELECT * FROM [PAR_2020_tab0b]"/>
   </connection>
 </connections>
@@ -240,9 +239,6 @@
     <t>#BED62F</t>
   </si>
   <si>
-    <t>#A70202</t>
-  </si>
-  <si>
     <t>#0F4D92</t>
   </si>
   <si>
@@ -361,13 +357,16 @@
   </si>
   <si>
     <t>MÁME TOHO DOSŤ</t>
+  </si>
+  <si>
+    <t>#cc001c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -878,48 +877,48 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20 % - zvýraznenie1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - zvýraznenie2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - zvýraznenie3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - zvýraznenie4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - zvýraznenie5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - zvýraznenie6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - zvýraznenie1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - zvýraznenie2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - zvýraznenie3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - zvýraznenie4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - zvýraznenie5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - zvýraznenie6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - zvýraznenie1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - zvýraznenie2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - zvýraznenie3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - zvýraznenie4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - zvýraznenie5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - zvýraznenie6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Dobrá" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Kontrolná bunka" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Nadpis 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Nadpis 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Nadpis 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Nadpis 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Neutrálna" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Poznámka" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Prepojená bunka" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Spolu" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Text upozornenia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Titul" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Vstup" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Výpočet" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Výstup" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Vysvetľujúci text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Zlá" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Zvýraznenie1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Zvýraznenie2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Zvýraznenie3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Zvýraznenie4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Zvýraznenie5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Zvýraznenie6" xfId="38" builtinId="49" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -972,7 +971,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternéÚdaje_2" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternéÚdaje_2" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="9" unboundColumnsRight="3">
     <queryTableFields count="8">
       <queryTableField id="1" name="Číslo politického subjektu" tableColumnId="1"/>
@@ -989,17 +988,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PAR_2020_tab0a" displayName="PAR_2020_tab0a" ref="A1:H26" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H26" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="PAR_2020_tab0a" displayName="PAR_2020_tab0a" ref="A1:H26" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H26"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Číslo politického subjektu" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Názov politického subjektu" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Oficiálna skratka politického subjektu" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Počet kandidátov" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Poznámka" queryTableFieldId="5" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{40C4F99E-B77A-405B-AF27-1CE4DA32FF5C}" uniqueName="6" name="image" queryTableFieldId="6" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{E807A2C5-2799-1341-AAD3-DE9F0F207977}" uniqueName="7" name="Farba" queryTableFieldId="7" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{D593BA0C-E992-1843-B4CC-34ADB33C68FC}" uniqueName="8" name="Skratka" queryTableFieldId="8" dataDxfId="0"/>
+    <tableColumn id="1" uniqueName="1" name="Číslo politického subjektu" queryTableFieldId="1"/>
+    <tableColumn id="2" uniqueName="2" name="Názov politického subjektu" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="3" uniqueName="3" name="Oficiálna skratka politického subjektu" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="4" uniqueName="4" name="Počet kandidátov" queryTableFieldId="4"/>
+    <tableColumn id="5" uniqueName="5" name="Poznámka" queryTableFieldId="5" dataDxfId="3"/>
+    <tableColumn id="6" uniqueName="6" name="image" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="7" uniqueName="7" name="Farba" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="8" uniqueName="8" name="Skratka" queryTableFieldId="8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1301,26 +1300,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="49" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1340,13 +1339,13 @@
         <v>66</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1366,13 +1365,13 @@
         <v>41</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1392,13 +1391,13 @@
         <v>42</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1418,13 +1417,13 @@
         <v>43</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1444,13 +1443,13 @@
         <v>44</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1470,13 +1469,13 @@
         <v>45</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1496,13 +1495,13 @@
         <v>46</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1522,13 +1521,13 @@
         <v>47</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1548,13 +1547,13 @@
         <v>48</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1574,13 +1573,13 @@
         <v>49</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1600,13 +1599,13 @@
         <v>50</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1629,10 +1628,10 @@
         <v>67</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1652,13 +1651,13 @@
         <v>52</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1678,13 +1677,13 @@
         <v>53</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1704,13 +1703,13 @@
         <v>54</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H15" s="6">
         <v>0.99</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1730,13 +1729,13 @@
         <v>55</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1756,13 +1755,13 @@
         <v>56</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1782,13 +1781,13 @@
         <v>57</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1808,13 +1807,13 @@
         <v>58</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1834,13 +1833,13 @@
         <v>59</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1860,13 +1859,13 @@
         <v>60</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1886,13 +1885,13 @@
         <v>61</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1912,13 +1911,13 @@
         <v>62</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1938,13 +1937,13 @@
         <v>63</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1964,13 +1963,13 @@
         <v>64</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1990,10 +1989,10 @@
         <v>65</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>